<commit_message>
Added "TEXT" to function BRfromMtext: TEXT needs to be in layers: 1506, 1507. br will be created in layers M1506, M1507 accordingly.
</commit_message>
<xml_diff>
--- a/Autocad/AddPoindWithCalcZ/check.xlsx
+++ b/Autocad/AddPoindWithCalcZ/check.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="22980" windowHeight="9555"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="4" r:id="rId1"/>
@@ -538,12 +538,12 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
@@ -570,13 +570,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>204100.64</v>
+        <v>204091.13</v>
       </c>
       <c r="C2">
-        <v>741347.32</v>
+        <v>741349.81</v>
       </c>
       <c r="D2">
-        <v>179.36</v>
+        <v>181.33</v>
       </c>
       <c r="F2">
         <f>D2-D3</f>
@@ -584,7 +584,7 @@
       </c>
       <c r="G2" s="1">
         <f>F2*G8/G7+D2</f>
-        <v>179.61438659294848</v>
+        <v>181.61392884305604</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -592,13 +592,13 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>204102.06</v>
+        <v>204095.88</v>
       </c>
       <c r="C3">
-        <v>741345.59</v>
+        <v>741350.14</v>
       </c>
       <c r="D3">
-        <v>178.74</v>
+        <v>180.71</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -606,10 +606,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>204101.36</v>
+        <v>204093.24</v>
       </c>
       <c r="C4">
-        <v>741346.75</v>
+        <v>741350.36</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -638,53 +638,53 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7">
         <f>B2-B3</f>
-        <v>-1.4199999999837019</v>
+        <v>-4.75</v>
       </c>
       <c r="C7">
         <f>B7*B7</f>
-        <v>2.0163999999537134</v>
+        <v>22.5625</v>
       </c>
       <c r="D7">
         <f>C2-C3</f>
-        <v>1.7299999999813735</v>
+        <v>-0.32999999995809048</v>
       </c>
       <c r="E7">
         <f>D7*D7</f>
-        <v>2.9928999999355526</v>
+        <v>0.10889999997233972</v>
       </c>
       <c r="F7">
         <f>C7+E7</f>
-        <v>5.009299999889266</v>
+        <v>22.671399999972341</v>
       </c>
       <c r="G7">
         <f>SQRT(F7)</f>
-        <v>2.2381465546047843</v>
+        <v>4.761449359173354</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8">
         <f>B2-B4</f>
-        <v>-0.71999999997206032</v>
+        <v>-2.1099999999860302</v>
       </c>
       <c r="C8">
         <f>B8*B8</f>
-        <v>0.51839999995976682</v>
+        <v>4.4520999999410469</v>
       </c>
       <c r="D8">
         <f>C2-C4</f>
-        <v>0.56999999994877726</v>
+        <v>-0.54999999993015081</v>
       </c>
       <c r="E8">
         <f>D8*D8</f>
-        <v>0.32489999994160607</v>
+        <v>0.3024999999231659</v>
       </c>
       <c r="F8">
         <f>C8+E8</f>
-        <v>0.84329999990137283</v>
+        <v>4.7545999998642126</v>
       </c>
       <c r="G8">
         <f>SQRT(F8)</f>
-        <v>0.91831367184713786</v>
+        <v>2.1805045287419635</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -705,9 +705,9 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -868,7 +868,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -880,7 +880,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>